<commit_message>
PO Testing Changes 04-03-2024
</commit_message>
<xml_diff>
--- a/DealerManagementSystem/Templates/Material.xlsx
+++ b/DealerManagementSystem/Templates/Material.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AJAX_ENGG\AJAXOneWeb\DealerManagementSystem\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEEC1E1-7115-47E5-8D8D-40D63C5B1A31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{156CA483-5170-45E9-931A-0B8FABDDC228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Projects" sheetId="2" r:id="rId1"/>
+    <sheet name="Material" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>